<commit_message>
added historical test data and historical pump data
</commit_message>
<xml_diff>
--- a/ga3_project/Tasks/IPS.XcelReporting/Results Overview/Results Overview.xlsx
+++ b/ga3_project/Tasks/IPS.XcelReporting/Results Overview/Results Overview.xlsx
@@ -45,15 +45,15 @@
     <t>Shell &amp; Tube Heat Exchanger - Tube Side - 0</t>
   </si>
   <si>
+    <t>Boundary Condition - 14</t>
+  </si>
+  <si>
+    <t>Pressure kPa</t>
+  </si>
+  <si>
     <t>Boundary Condition - 18</t>
   </si>
   <si>
-    <t>Boundary Condition - 14</t>
-  </si>
-  <si>
-    <t>Pressure kPa</t>
-  </si>
-  <si>
     <t>Identifier</t>
   </si>
   <si>
@@ -90,43 +90,43 @@
     <t>Node - 4</t>
   </si>
   <si>
+    <t>Boundary Condition - 19</t>
+  </si>
+  <si>
+    <t>Static pressure kPa</t>
+  </si>
+  <si>
+    <t>Total pressure kPa</t>
+  </si>
+  <si>
+    <t>Node - 24</t>
+  </si>
+  <si>
+    <t>Node - 17</t>
+  </si>
+  <si>
     <t>Nozzle - 20 Copy(002)</t>
   </si>
   <si>
-    <t>Static pressure kPa</t>
-  </si>
-  <si>
-    <t>Total pressure kPa</t>
-  </si>
-  <si>
-    <t>Node - 24</t>
-  </si>
-  <si>
-    <t>Node - 17</t>
-  </si>
-  <si>
     <t>Quality</t>
   </si>
   <si>
-    <t>Boundary Condition - 19</t>
-  </si>
-  <si>
     <t>Total heat transfer kW</t>
   </si>
   <si>
     <t>Total temperature °C</t>
   </si>
   <si>
+    <t>Node - 21</t>
+  </si>
+  <si>
+    <t>Boundary Condition - 16</t>
+  </si>
+  <si>
+    <t>Temperature °C</t>
+  </si>
+  <si>
     <t>Node - 10</t>
-  </si>
-  <si>
-    <t>Temperature °C</t>
-  </si>
-  <si>
-    <t>Boundary Condition - 16</t>
-  </si>
-  <si>
-    <t>Node - 21</t>
   </si>
   <si>
     <t>Total volume flow m³/s</t>
@@ -624,81 +624,81 @@
         <v>11</v>
       </c>
       <c s="2" t="s">
+        <v>9</v>
+      </c>
+      <c s="2" t="s">
+        <v>34</v>
+      </c>
+      <c s="2" t="s">
+        <v>20</v>
+      </c>
+      <c s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>8</v>
+      </c>
+      <c s="1">
+        <v>101</v>
+      </c>
+      <c s="1">
+        <v>20</v>
+      </c>
+      <c s="1">
+        <v>0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>33</v>
+      </c>
+      <c s="1">
+        <v>101</v>
+      </c>
+      <c s="1">
+        <v>60</v>
+      </c>
+      <c s="1">
+        <v>0.40789128016877202</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
         <v>10</v>
       </c>
-      <c s="2" t="s">
-        <v>33</v>
-      </c>
-      <c s="2" t="s">
-        <v>20</v>
-      </c>
-      <c s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>9</v>
-      </c>
       <c s="1">
         <v>101</v>
       </c>
       <c s="1">
-        <v>20</v>
-      </c>
-      <c s="1">
-        <v>0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>34</v>
+        <v>26.758478073313881</v>
+      </c>
+      <c s="1">
+        <v>-0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>23</v>
       </c>
       <c s="1">
         <v>101</v>
       </c>
       <c s="1">
-        <v>60</v>
-      </c>
-      <c s="1">
-        <v>0.45715376667850405</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>8</v>
-      </c>
-      <c s="1">
-        <v>101</v>
-      </c>
-      <c s="1">
-        <v>27.719104893092322</v>
-      </c>
-      <c s="1">
-        <v>-0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>29</v>
-      </c>
-      <c s="1">
-        <v>101</v>
-      </c>
-      <c s="1">
-        <v>51.199297333859533</v>
-      </c>
-      <c s="1">
-        <v>-0.45715376667850405</v>
+        <v>50.410472697096395</v>
+      </c>
+      <c s="1">
+        <v>-0.40789128016877202</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -771,16 +771,16 @@
         <v>38</v>
       </c>
       <c s="1">
-        <v>0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>5.2294615651482328E-04</v>
-      </c>
-      <c s="1">
-        <v>117.48735085809166</v>
-      </c>
-      <c s="1">
-        <v>-32.974701716183304</v>
+        <v>0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>5.8071369843295736E-04</v>
+      </c>
+      <c s="1">
+        <v>114.54668815168121</v>
+      </c>
+      <c s="1">
+        <v>-27.093376303362412</v>
       </c>
       <c s="1">
         <v>19.999999984029216</v>
@@ -798,7 +798,7 @@
         <v>0</v>
       </c>
       <c s="1">
-        <v>-0.017243985699948727</v>
+        <v>-0.015733489546232583</v>
       </c>
     </row>
     <row>
@@ -806,16 +806,16 @@
         <v>6</v>
       </c>
       <c s="1">
-        <v>0.45715376667850405</v>
-      </c>
-      <c s="1">
-        <v>4.6497918030279838E-04</v>
-      </c>
-      <c s="1">
-        <v>104.28529551223266</v>
-      </c>
-      <c s="1">
-        <v>-6.5705910244653207</v>
+        <v>0.40789128016877202</v>
+      </c>
+      <c s="1">
+        <v>4.1487343412597281E-04</v>
+      </c>
+      <c s="1">
+        <v>108.1402930354303</v>
+      </c>
+      <c s="1">
+        <v>-14.280586070860634</v>
       </c>
       <c s="1">
         <v>60.000000050343715</v>
@@ -833,7 +833,7 @@
         <v>0</v>
       </c>
       <c s="1">
-        <v>-3.0551870635795297E-03</v>
+        <v>-5.9246353057268485E-03</v>
       </c>
     </row>
   </sheetData>
@@ -876,7 +876,7 @@
         <v>20</v>
       </c>
       <c s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c s="2" t="s">
         <v>4</v>
@@ -884,53 +884,99 @@
     </row>
     <row>
       <c s="1" t="s">
+        <v>35</v>
+      </c>
+      <c s="1">
+        <v>101.87453747771652</v>
+      </c>
+      <c s="1">
+        <v>101.14302367685772</v>
+      </c>
+      <c s="1">
+        <v>50.410304088537032</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>5</v>
+      </c>
+      <c s="1">
+        <v>101</v>
+      </c>
+      <c s="1">
+        <v>101</v>
+      </c>
+      <c s="1">
+        <v>20</v>
+      </c>
+      <c s="1">
+        <v>0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>27</v>
+      </c>
+      <c s="1">
+        <v>101</v>
+      </c>
+      <c s="1">
+        <v>101</v>
+      </c>
+      <c s="1">
+        <v>60</v>
+      </c>
+      <c s="1">
+        <v>0.40789128016877202</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
         <v>32</v>
       </c>
       <c s="1">
-        <v>102.09733898979442</v>
-      </c>
-      <c s="1">
-        <v>101.90151588535339</v>
-      </c>
-      <c s="1">
-        <v>51.199086994422544</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>5</v>
-      </c>
-      <c s="1">
         <v>101</v>
       </c>
       <c s="1">
         <v>101</v>
       </c>
       <c s="1">
-        <v>20</v>
-      </c>
-      <c s="1">
-        <v>0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>27</v>
+        <v>26.758478073313881</v>
+      </c>
+      <c s="1">
+        <v>-0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>1</v>
       </c>
       <c s="1">
         <v>101</v>
@@ -939,56 +985,10 @@
         <v>101</v>
       </c>
       <c s="1">
-        <v>60</v>
-      </c>
-      <c s="1">
-        <v>0.45715376667850405</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>35</v>
-      </c>
-      <c s="1">
-        <v>101</v>
-      </c>
-      <c s="1">
-        <v>101</v>
-      </c>
-      <c s="1">
-        <v>27.719104893092322</v>
-      </c>
-      <c s="1">
-        <v>-0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>1</v>
-      </c>
-      <c s="1">
-        <v>101</v>
-      </c>
-      <c s="1">
-        <v>101</v>
-      </c>
-      <c s="1">
-        <v>51.199297333859533</v>
-      </c>
-      <c s="1">
-        <v>-0.45715376667850405</v>
+        <v>50.410472697096395</v>
+      </c>
+      <c s="1">
+        <v>-0.40789128016877202</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1002,13 +1002,13 @@
         <v>13</v>
       </c>
       <c s="1">
-        <v>133.97470171618332</v>
-      </c>
-      <c s="1">
-        <v>133.97470171618332</v>
-      </c>
-      <c s="1">
-        <v>20.000463037545728</v>
+        <v>128.09337630336242</v>
+      </c>
+      <c s="1">
+        <v>128.09337630336242</v>
+      </c>
+      <c s="1">
+        <v>20.00038042140045</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1025,13 +1025,13 @@
         <v>26</v>
       </c>
       <c s="1">
-        <v>107.57059102446532</v>
-      </c>
-      <c s="1">
-        <v>107.57059102446532</v>
-      </c>
-      <c s="1">
-        <v>60.000200026189873</v>
+        <v>115.28058607086064</v>
+      </c>
+      <c s="1">
+        <v>115.28058607086064</v>
+      </c>
+      <c s="1">
+        <v>60.000434616610619</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1048,13 +1048,13 @@
         <v>22</v>
       </c>
       <c s="1">
-        <v>132.55041711223396</v>
-      </c>
-      <c s="1">
-        <v>132.55041711223396</v>
-      </c>
-      <c s="1">
-        <v>20.000783769656209</v>
+        <v>126.33952836168515</v>
+      </c>
+      <c s="1">
+        <v>126.33952836168515</v>
+      </c>
+      <c s="1">
+        <v>20.000775369058886</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1071,13 +1071,13 @@
         <v>2</v>
       </c>
       <c s="1">
-        <v>102.42376700087829</v>
-      </c>
-      <c s="1">
-        <v>102.42376700087829</v>
-      </c>
-      <c s="1">
-        <v>27.718793915278411</v>
+        <v>102.75343926245225</v>
+      </c>
+      <c s="1">
+        <v>102.66161965939511</v>
+      </c>
+      <c s="1">
+        <v>26.758093477231228</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1094,13 +1094,13 @@
         <v>21</v>
       </c>
       <c s="1">
-        <v>106.47005633734477</v>
-      </c>
-      <c s="1">
-        <v>106.27338832930455</v>
-      </c>
-      <c s="1">
-        <v>60.000434131303621</v>
+        <v>114.40340156297715</v>
+      </c>
+      <c s="1">
+        <v>113.66841155205599</v>
+      </c>
+      <c s="1">
+        <v>60.000621214731439</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1179,22 +1179,22 @@
         <v>3</v>
       </c>
       <c s="1">
-        <v>0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>5.2293773067470771E-04</v>
-      </c>
-      <c s="1">
-        <v>133.26255941420862</v>
-      </c>
-      <c s="1">
-        <v>1.4242846039493451</v>
-      </c>
-      <c s="1">
-        <v>20.000463037545728</v>
-      </c>
-      <c s="1">
-        <v>998.16857274907409</v>
+        <v>0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>5.8070601064659022E-04</v>
+      </c>
+      <c s="1">
+        <v>127.21645233252379</v>
+      </c>
+      <c s="1">
+        <v>1.7538479416772608</v>
+      </c>
+      <c s="1">
+        <v>20.00038042140045</v>
+      </c>
+      <c s="1">
+        <v>998.16570423299493</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1214,57 +1214,57 @@
         <v>37</v>
       </c>
       <c s="1">
-        <v>0.45715376667850405</v>
-      </c>
-      <c s="1">
-        <v>4.6497798365264717E-04</v>
-      </c>
-      <c s="1">
-        <v>107.02032368090504</v>
-      </c>
-      <c s="1">
-        <v>1.1005346871205548</v>
-      </c>
-      <c s="1">
-        <v>60.000200026189873</v>
-      </c>
-      <c s="1">
-        <v>983.17293022357671</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row>
-      <c s="1" t="s">
-        <v>23</v>
-      </c>
-      <c s="1">
-        <v>0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>5.2396545358731044E-04</v>
-      </c>
-      <c s="1">
-        <v>101.71188350043914</v>
-      </c>
-      <c s="1">
-        <v>1.4237670008782879</v>
-      </c>
-      <c s="1">
-        <v>27.718793915278411</v>
-      </c>
-      <c s="1">
-        <v>996.21073149595168</v>
+        <v>0.40789128016877202</v>
+      </c>
+      <c s="1">
+        <v>4.1487111357199711E-04</v>
+      </c>
+      <c s="1">
+        <v>114.8419938169189</v>
+      </c>
+      <c s="1">
+        <v>0.87718450788348856</v>
+      </c>
+      <c s="1">
+        <v>60.000434616610619</v>
+      </c>
+      <c s="1">
+        <v>983.17589927228903</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row>
+      <c s="1" t="s">
+        <v>28</v>
+      </c>
+      <c s="1">
+        <v>0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>5.8169684201882991E-04</v>
+      </c>
+      <c s="1">
+        <v>101.87671963122612</v>
+      </c>
+      <c s="1">
+        <v>1.7534392624522444</v>
+      </c>
+      <c s="1">
+        <v>26.758093477231228</v>
+      </c>
+      <c s="1">
+        <v>996.46548194816501</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1284,22 +1284,22 @@
         <v>14</v>
       </c>
       <c s="1">
-        <v>0.45715376667850405</v>
-      </c>
-      <c s="1">
-        <v>4.6294835808668392E-04</v>
-      </c>
-      <c s="1">
-        <v>101.54866949489721</v>
-      </c>
-      <c s="1">
-        <v>1.097338989794429</v>
-      </c>
-      <c s="1">
-        <v>51.199086994422544</v>
-      </c>
-      <c s="1">
-        <v>987.48328630832884</v>
+        <v>0.40789128016877202</v>
+      </c>
+      <c s="1">
+        <v>4.129159007210742E-04</v>
+      </c>
+      <c s="1">
+        <v>101.43726873885825</v>
+      </c>
+      <c s="1">
+        <v>0.87453747771651247</v>
+      </c>
+      <c s="1">
+        <v>50.410304088537032</v>
+      </c>
+      <c s="1">
+        <v>987.83137057736292</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1381,31 +1381,31 @@
         <v>17</v>
       </c>
       <c s="1">
-        <v>0.52198000826255353</v>
-      </c>
-      <c s="1">
-        <v>5.2294534122572652E-04</v>
-      </c>
-      <c s="1">
-        <v>117.48709205655612</v>
-      </c>
-      <c s="1">
-        <v>30.126650111355673</v>
-      </c>
-      <c s="1">
-        <v>23.787161601861442</v>
-      </c>
-      <c s="1">
-        <v>997.25285372361896</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>0</v>
-      </c>
-      <c s="1">
-        <v>16.832452209838348</v>
+        <v>0.57964082406946782</v>
+      </c>
+      <c s="1">
+        <v>5.8072511503463257E-04</v>
+      </c>
+      <c s="1">
+        <v>114.5464838120687</v>
+      </c>
+      <c s="1">
+        <v>23.586089099232908</v>
+      </c>
+      <c s="1">
+        <v>23.448429779509638</v>
+      </c>
+      <c s="1">
+        <v>997.34082971372038</v>
+      </c>
+      <c s="1">
+        <v>0</v>
+      </c>
+      <c s="1">
+        <v>0.85858160453074872</v>
+      </c>
+      <c s="1">
+        <v>16.367217883399693</v>
       </c>
       <c s="1">
         <v>0</v>
@@ -1478,31 +1478,31 @@
         <v>7</v>
       </c>
       <c s="1">
-        <v>0.45715376667850399</v>
-      </c>
-      <c s="1">
-        <v>4.6489581059473467E-04</v>
-      </c>
-      <c s="1">
-        <v>104.28369766356958</v>
-      </c>
-      <c s="1">
-        <v>4.3727173475503367</v>
-      </c>
-      <c s="1">
-        <v>55.516913834223033</v>
-      </c>
-      <c s="1">
-        <v>985.36635600201294</v>
-      </c>
-      <c s="1">
-        <v>1.2650970299795317</v>
-      </c>
-      <c s="1">
-        <v>1.2588800191700404</v>
-      </c>
-      <c s="1">
-        <v>-16.832452209827863</v>
+        <v>0.40789128016877202</v>
+      </c>
+      <c s="1">
+        <v>4.1481526107133791E-04</v>
+      </c>
+      <c s="1">
+        <v>108.13896952034683</v>
+      </c>
+      <c s="1">
+        <v>12.528864085260633</v>
+      </c>
+      <c s="1">
+        <v>54.559011297276527</v>
+      </c>
+      <c s="1">
+        <v>985.83626221621535</v>
+      </c>
+      <c s="1">
+        <v>2.4455146003733672</v>
+      </c>
+      <c s="1">
+        <v>2.4339682540425231</v>
+      </c>
+      <c s="1">
+        <v>-16.367217883704463</v>
       </c>
       <c s="1">
         <v>0</v>

</xml_diff>